<commit_message>
cambios carlos documentos y texto
</commit_message>
<xml_diff>
--- a/Estimacion de tiempo.xlsx
+++ b/Estimacion de tiempo.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caili\Desktop\laboratorio1Act\proyectoCompiladoresIISemestre2019\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7F55E3-7AA1-43DE-8BB7-F1D6AB3C2913}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -60,14 +54,14 @@
     <t>Diseñar mensajes de error</t>
   </si>
   <si>
-    <t>*</t>
+    <t>**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -200,7 +194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -377,27 +371,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="69" customWidth="1"/>
     <col min="2" max="2" width="88.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,7 +399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -413,7 +407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -421,7 +415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -429,7 +423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -437,7 +431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Documentos de especificación y estimación time
Cambios en ambos de documentos
</commit_message>
<xml_diff>
--- a/Estimacion de tiempo.xlsx
+++ b/Estimacion de tiempo.xlsx
@@ -1,26 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollar gramatica y documentar la discusión </t>
+  </si>
+  <si>
+    <t>2 horas</t>
+  </si>
+  <si>
+    <t>Transformar gramática a una gramática LL</t>
+  </si>
+  <si>
+    <t>4 horas</t>
+  </si>
+  <si>
+    <t>Implementar scanner</t>
+  </si>
+  <si>
+    <t>6 horas</t>
+  </si>
+  <si>
+    <t>Crear conjunto de pruebas</t>
+  </si>
+  <si>
+    <t>1 hora</t>
+  </si>
+  <si>
+    <t>Diseñar mensajes de error</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -29,12 +70,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -111,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -146,7 +194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -323,20 +371,75 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="69" customWidth="1"/>
+    <col min="2" max="2" width="88.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>